<commit_message>
Removed unnecessary table column
</commit_message>
<xml_diff>
--- a/src/_posts/chaos-engineering/chaos-engineering-through-staged-resiliency/notes/playbooks.xlsx
+++ b/src/_posts/chaos-engineering/chaos-engineering-through-staged-resiliency/notes/playbooks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\Gremlin\gremlin-projects\gremlin-blog-posts\src\_posts\chaos-engineering\chaos-engineering-through-staged-resiliency\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E30DC8-1F2D-4E7F-9DB2-0B13108C5DB2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFB33E2-A0E9-44C8-9B30-D468FAA73F18}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21825" windowHeight="12750" activeTab="2" xr2:uid="{3DED6E99-5CD8-4F84-8CE0-E34B0D49F942}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
   <si>
     <t>Criticality Period</t>
   </si>
@@ -807,10 +807,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F24DCD-F00C-4962-8AF9-AAFB07396828}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F3"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,11 +820,10 @@
     <col min="3" max="3" width="67.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -840,11 +839,8 @@
       <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -860,11 +856,8 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -879,9 +872,6 @@
       </c>
       <c r="E3">
         <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>